<commit_message>
HKDON: flat extrapolation for contribution (2)
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD/HKD_MxContributor.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD/HKD_MxContributor.xlsx
@@ -430,7 +430,7 @@
     <numFmt numFmtId="171" formatCode="0.E+00"/>
     <numFmt numFmtId="172" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,6 +530,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -1099,12 +1105,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1165,6 +1165,12 @@
     </xf>
     <xf numFmtId="172" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1488,6 +1494,8 @@
 HKD6M1X7F=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AG15" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>0.23686000000000001</v>
         <stp/>
@@ -2019,6 +2027,8 @@
         <stp xml:space="preserve">	HKD3M18M=_x0003_BID_x0007_DTSIMI1ÿ_x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</stp>
         <tr r="AE21" s="7"/>
       </tp>
+    </main>
+    <main first="pldatasource.rtgetrtdserver">
       <tp>
         <v>2.0100000000000002</v>
         <stp/>
@@ -2414,7 +2424,7 @@
       <sheetData sheetId="0">
         <row r="22">
           <cell r="D22">
-            <v>3</v>
+            <v>7</v>
           </cell>
         </row>
       </sheetData>
@@ -2903,9 +2913,7 @@
       <c r="C4" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="60">
-        <v>42129.442453703705</v>
-      </c>
+      <c r="D4" s="60"/>
       <c r="E4" s="59"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2970,7 +2978,7 @@
       </c>
       <c r="D6" s="61">
         <f>[1]!TriggerCounter</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E6" s="59"/>
       <c r="F6" s="2"/>
@@ -8361,7 +8369,7 @@
       <c r="BL20" s="2"/>
       <c r="BM20" s="2"/>
     </row>
-    <row r="21" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="106" t="s">
         <v>48</v>
       </c>
@@ -8429,11 +8437,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS18MD=</v>
       </c>
-      <c r="V21" s="109">
+      <c r="V21" s="130">
         <f>$V$20</f>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W21" s="109">
+      <c r="W21" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -8502,7 +8510,7 @@
       <c r="BL21" s="2"/>
       <c r="BM21" s="2"/>
     </row>
-    <row r="22" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="106" t="s">
         <v>24</v>
       </c>
@@ -8529,7 +8537,7 @@
       <c r="G22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="128" t="str">
+      <c r="H22" s="126" t="str">
         <f t="shared" ref="H22:H29" si="15">A22</f>
         <v>2Y</v>
       </c>
@@ -8584,11 +8592,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS2YD=</v>
       </c>
-      <c r="V22" s="109">
+      <c r="V22" s="130">
         <f t="shared" ref="V22:V29" si="17">$V$20</f>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W22" s="109">
+      <c r="W22" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -8681,7 +8689,7 @@
       <c r="BL22" s="2"/>
       <c r="BM22" s="2"/>
     </row>
-    <row r="23" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="106" t="s">
         <v>25</v>
       </c>
@@ -8708,7 +8716,7 @@
       <c r="G23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="128" t="str">
+      <c r="H23" s="126" t="str">
         <f t="shared" si="15"/>
         <v>3Y</v>
       </c>
@@ -8764,11 +8772,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS3YD=</v>
       </c>
-      <c r="V23" s="109">
+      <c r="V23" s="130">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W23" s="109">
+      <c r="W23" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -8861,7 +8869,7 @@
       <c r="BL23" s="2"/>
       <c r="BM23" s="2"/>
     </row>
-    <row r="24" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="106" t="s">
         <v>26</v>
       </c>
@@ -8888,7 +8896,7 @@
       <c r="G24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="128" t="str">
+      <c r="H24" s="126" t="str">
         <f t="shared" si="15"/>
         <v>4Y</v>
       </c>
@@ -8944,11 +8952,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS4YD=</v>
       </c>
-      <c r="V24" s="109">
+      <c r="V24" s="130">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W24" s="109">
+      <c r="W24" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -9041,7 +9049,7 @@
       <c r="BL24" s="2"/>
       <c r="BM24" s="2"/>
     </row>
-    <row r="25" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="106" t="s">
         <v>27</v>
       </c>
@@ -9068,7 +9076,7 @@
       <c r="G25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="128" t="str">
+      <c r="H25" s="126" t="str">
         <f t="shared" si="15"/>
         <v>5Y</v>
       </c>
@@ -9124,11 +9132,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS5YD=</v>
       </c>
-      <c r="V25" s="109">
+      <c r="V25" s="130">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W25" s="109">
+      <c r="W25" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -9221,7 +9229,7 @@
       <c r="BL25" s="2"/>
       <c r="BM25" s="2"/>
     </row>
-    <row r="26" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:65" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="106" t="s">
         <v>28</v>
       </c>
@@ -9248,7 +9256,7 @@
       <c r="G26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="128" t="str">
+      <c r="H26" s="126" t="str">
         <f t="shared" si="15"/>
         <v>7Y</v>
       </c>
@@ -9304,11 +9312,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS7YD=</v>
       </c>
-      <c r="V26" s="109">
+      <c r="V26" s="130">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W26" s="109">
+      <c r="W26" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -9401,7 +9409,7 @@
       <c r="BL26" s="2"/>
       <c r="BM26" s="2"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:65" ht="12" x14ac:dyDescent="0.25">
       <c r="A27" s="106" t="s">
         <v>29</v>
       </c>
@@ -9428,7 +9436,7 @@
       <c r="G27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="128" t="str">
+      <c r="H27" s="126" t="str">
         <f t="shared" si="15"/>
         <v>10Y</v>
       </c>
@@ -9484,11 +9492,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS10YD=</v>
       </c>
-      <c r="V27" s="109">
+      <c r="V27" s="130">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W27" s="109">
+      <c r="W27" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -9581,7 +9589,7 @@
       <c r="BL27" s="2"/>
       <c r="BM27" s="2"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:65" ht="12" x14ac:dyDescent="0.25">
       <c r="A28" s="106" t="s">
         <v>30</v>
       </c>
@@ -9608,7 +9616,7 @@
       <c r="G28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="128" t="str">
+      <c r="H28" s="126" t="str">
         <f t="shared" si="15"/>
         <v>12Y</v>
       </c>
@@ -9664,11 +9672,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS12YD=</v>
       </c>
-      <c r="V28" s="109">
+      <c r="V28" s="130">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W28" s="109">
+      <c r="W28" s="130">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -9761,7 +9769,7 @@
       <c r="BL28" s="2"/>
       <c r="BM28" s="2"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:65" ht="12" x14ac:dyDescent="0.25">
       <c r="A29" s="107" t="s">
         <v>31</v>
       </c>
@@ -9788,7 +9796,7 @@
       <c r="G29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="129" t="str">
+      <c r="H29" s="127" t="str">
         <f t="shared" si="15"/>
         <v>15Y</v>
       </c>
@@ -9844,11 +9852,11 @@
         <f t="shared" si="14"/>
         <v>HKDOIS15YD=</v>
       </c>
-      <c r="V29" s="110">
+      <c r="V29" s="131">
         <f t="shared" si="17"/>
         <v>0.14999999998094102</v>
       </c>
-      <c r="W29" s="110">
+      <c r="W29" s="131">
         <f t="shared" si="10"/>
         <v>0.14999999998094102</v>
       </c>
@@ -14150,7 +14158,7 @@
       <c r="L6" s="38"/>
       <c r="M6" s="78" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00219#0000</v>
+        <v>obj_0021a#0001</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="b">
@@ -14206,7 +14214,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00209#0000</v>
+        <v>obj_00214#0001</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -14256,7 +14264,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001fb#0000</v>
+        <v>obj_001f0#0001</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -14306,7 +14314,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="108" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001e2#0000</v>
+        <v>obj_001e4#0001</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -14392,7 +14400,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="78" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D11,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c3#0000</v>
+        <v>obj_00200#0001</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="77" t="s">
@@ -14445,7 +14453,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D12,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ee#0000</v>
+        <v>obj_001e7#0001</v>
       </c>
       <c r="N12" s="38"/>
       <c r="O12" s="79"/>
@@ -14492,7 +14500,7 @@
       <c r="L13" s="38"/>
       <c r="M13" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D13,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c5#0000</v>
+        <v>obj_001c3#0001</v>
       </c>
       <c r="N13" s="38"/>
       <c r="O13" s="79"/>
@@ -14542,7 +14550,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D14,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ce#0000</v>
+        <v>obj_001f9#0001</v>
       </c>
       <c r="N14" s="38"/>
       <c r="O14" s="79"/>
@@ -14589,7 +14597,7 @@
       <c r="L15" s="38"/>
       <c r="M15" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D15,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d4#0000</v>
+        <v>obj_001f2#0001</v>
       </c>
       <c r="N15" s="38"/>
       <c r="O15" s="79"/>
@@ -14636,7 +14644,7 @@
       <c r="L16" s="38"/>
       <c r="M16" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D16,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020b#0000</v>
+        <v>obj_001ce#0001</v>
       </c>
       <c r="N16" s="38"/>
       <c r="O16" s="79"/>
@@ -14686,7 +14694,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D17,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c6#0000</v>
+        <v>obj_001d3#0001</v>
       </c>
       <c r="N17" s="75"/>
       <c r="O17" s="79"/>
@@ -14733,7 +14741,7 @@
       <c r="L18" s="38"/>
       <c r="M18" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D18,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e9#0000</v>
+        <v>obj_001fa#0001</v>
       </c>
       <c r="N18" s="75"/>
       <c r="O18" s="79"/>
@@ -14780,7 +14788,7 @@
       <c r="L19" s="38"/>
       <c r="M19" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D19,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001db#0000</v>
+        <v>obj_00204#0001</v>
       </c>
       <c r="N19" s="75"/>
       <c r="O19" s="79"/>
@@ -14830,7 +14838,7 @@
       <c r="L20" s="38"/>
       <c r="M20" s="27" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D20,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001eb#0000</v>
+        <v>obj_001c8#0001</v>
       </c>
       <c r="N20" s="75"/>
       <c r="O20" s="79"/>
@@ -14853,18 +14861,18 @@
       <c r="D21" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="119" t="s">
+      <c r="E21" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="120">
+      <c r="F21" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G21" s="120">
+      <c r="G21" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M21,F21,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H21" s="120">
+      <c r="H21" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M21,G21,Trigger)</f>
         <v>42681</v>
       </c>
@@ -14874,10 +14882,10 @@
       </c>
       <c r="J21" s="51"/>
       <c r="K21" s="51"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="117" t="str">
+      <c r="L21" s="114"/>
+      <c r="M21" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D21,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f3#0000</v>
+        <v>obj_00211#0001</v>
       </c>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -14900,18 +14908,18 @@
       <c r="D22" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="119" t="s">
+      <c r="E22" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="120">
+      <c r="F22" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G22" s="120">
+      <c r="G22" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M22,F22,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H22" s="120">
+      <c r="H22" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M22,G22,Trigger)</f>
         <v>42863</v>
       </c>
@@ -14924,10 +14932,10 @@
         <v>HKD1M2Y=</v>
       </c>
       <c r="K22" s="51"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="117" t="str">
+      <c r="L22" s="114"/>
+      <c r="M22" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00208#0000</v>
+        <v>obj_001e2#0001</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="79"/>
@@ -14950,18 +14958,18 @@
       <c r="D23" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="119" t="s">
+      <c r="E23" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="120">
+      <c r="F23" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G23" s="120">
+      <c r="G23" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M23,F23,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H23" s="120">
+      <c r="H23" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M23,G23,Trigger)</f>
         <v>43227</v>
       </c>
@@ -14974,10 +14982,10 @@
         <v>HKD1M3Y=</v>
       </c>
       <c r="K23" s="51"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117" t="str">
+      <c r="L23" s="114"/>
+      <c r="M23" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ca#0000</v>
+        <v>obj_001c4#0001</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -15000,18 +15008,18 @@
       <c r="D24" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="120">
+      <c r="F24" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G24" s="120">
+      <c r="G24" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M24,F24,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H24" s="120">
+      <c r="H24" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M24,G24,Trigger)</f>
         <v>43591</v>
       </c>
@@ -15024,10 +15032,10 @@
         <v>HKD1M4Y=</v>
       </c>
       <c r="K24" s="51"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="117" t="str">
+      <c r="L24" s="114"/>
+      <c r="M24" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001de#0000</v>
+        <v>obj_001c6#0001</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -15050,18 +15058,18 @@
       <c r="D25" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="E25" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="120">
+      <c r="F25" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G25" s="120">
+      <c r="G25" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M25,F25,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H25" s="120">
+      <c r="H25" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M25,G25,Trigger)</f>
         <v>43957</v>
       </c>
@@ -15074,10 +15082,10 @@
         <v>HKD1M5Y=</v>
       </c>
       <c r="K25" s="51"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="117" t="str">
+      <c r="L25" s="114"/>
+      <c r="M25" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f0#0000</v>
+        <v>obj_001eb#0001</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -15100,18 +15108,18 @@
       <c r="D26" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="120">
+      <c r="F26" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G26" s="120">
+      <c r="G26" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M26,F26,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H26" s="120">
+      <c r="H26" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M26,G26,Trigger)</f>
         <v>44687</v>
       </c>
@@ -15124,10 +15132,10 @@
         <v>HKD1M7Y=</v>
       </c>
       <c r="K26" s="51"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="117" t="str">
+      <c r="L26" s="114"/>
+      <c r="M26" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e1#0000</v>
+        <v>obj_001f3#0001</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -15150,18 +15158,18 @@
       <c r="D27" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="120">
+      <c r="F27" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G27" s="120">
+      <c r="G27" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M27,F27,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H27" s="120">
+      <c r="H27" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M27,G27,Trigger)</f>
         <v>45783</v>
       </c>
@@ -15174,10 +15182,10 @@
         <v>HKD1M10Y=</v>
       </c>
       <c r="K27" s="51"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="117" t="str">
+      <c r="L27" s="114"/>
+      <c r="M27" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00201#0000</v>
+        <v>obj_001d8#0001</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -15200,18 +15208,18 @@
       <c r="D28" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="119" t="s">
+      <c r="E28" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="120">
+      <c r="F28" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G28" s="120">
+      <c r="G28" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M28,F28,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H28" s="120">
+      <c r="H28" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M28,G28,Trigger)</f>
         <v>46513</v>
       </c>
@@ -15224,10 +15232,10 @@
         <v>HKD1M12Y=</v>
       </c>
       <c r="K28" s="51"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="117" t="str">
+      <c r="L28" s="114"/>
+      <c r="M28" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001da#0000</v>
+        <v>obj_001dd#0001</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -15250,18 +15258,18 @@
       <c r="D29" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="122" t="s">
+      <c r="E29" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="123">
+      <c r="F29" s="121">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G29" s="123">
+      <c r="G29" s="121">
         <f>_xll.qlInterestRateIndexValueDate(M29,F29,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H29" s="123">
+      <c r="H29" s="121">
         <f>_xll.qlInterestRateIndexMaturity(M29,G29,Trigger)</f>
         <v>47609</v>
       </c>
@@ -15269,15 +15277,15 @@
         <f>_xll.qlIndexFixing(M29,F29,TRUE,AllTriggers)</f>
         <v>2.147285741941456E-2</v>
       </c>
-      <c r="J29" s="125" t="str">
+      <c r="J29" s="123" t="str">
         <f>Contribution!I29</f>
         <v>HKD1M15Y=</v>
       </c>
-      <c r="K29" s="125"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="126" t="str">
+      <c r="K29" s="123"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="124" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001dd#0000</v>
+        <v>obj_00217#0001</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -18266,8 +18274,8 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="38"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23" t="s">
         <v>39</v>
@@ -18316,8 +18324,8 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="38"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
       <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
@@ -18348,7 +18356,7 @@
       <c r="L6" s="38"/>
       <c r="M6" s="78" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d6#0000</v>
+        <v>obj_001ff#0001</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="b">
@@ -18372,8 +18380,8 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="18" t="s">
         <v>78</v>
       </c>
@@ -18404,7 +18412,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001dc#0000</v>
+        <v>obj_0020f#0001</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -18422,8 +18430,8 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="38"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="18" t="s">
         <v>16</v>
       </c>
@@ -18454,7 +18462,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001ef#0000</v>
+        <v>obj_001c9#0001</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -18472,8 +18480,8 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="38"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="18" t="s">
         <v>17</v>
       </c>
@@ -18504,7 +18512,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001f9#0000</v>
+        <v>obj_00212#0001</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -18522,8 +18530,8 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="38"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="18" t="s">
         <v>18</v>
       </c>
@@ -18551,7 +18559,7 @@
       <c r="L10" s="38"/>
       <c r="M10" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D10="ON",D10="TN",D10="SN"),"1D",IF(D10="SW","1W",D10)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001c4#0000</v>
+        <v>obj_0020c#0001</v>
       </c>
       <c r="N10" s="75"/>
       <c r="O10" s="79"/>
@@ -18569,8 +18577,8 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="38"/>
-      <c r="B11" s="114"/>
-      <c r="C11" s="114"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="112"/>
       <c r="D11" s="19" t="s">
         <v>19</v>
       </c>
@@ -18601,7 +18609,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="29" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D11="ON",D11="TN",D11="SN"),"1D",IF(D11="SW","1W",D11)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001cd#0000</v>
+        <v>obj_00202#0001</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="79"/>
@@ -18619,10 +18627,10 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="38"/>
-      <c r="B12" s="113">
+      <c r="B12" s="111">
         <v>1</v>
       </c>
-      <c r="C12" s="113" t="s">
+      <c r="C12" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D12" s="18" t="s">
@@ -18635,7 +18643,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G12,Trigger)</f>
         <v>42163</v>
       </c>
-      <c r="G12" s="120">
+      <c r="G12" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B12&amp;"M","mf",TRUE)</f>
         <v>42163</v>
       </c>
@@ -18670,10 +18678,10 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="38"/>
-      <c r="B13" s="113">
+      <c r="B13" s="111">
         <v>2</v>
       </c>
-      <c r="C13" s="113" t="s">
+      <c r="C13" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -18686,7 +18694,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G13,Trigger)</f>
         <v>42192</v>
       </c>
-      <c r="G13" s="120">
+      <c r="G13" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B13&amp;"M","mf",TRUE)</f>
         <v>42192</v>
       </c>
@@ -18718,10 +18726,10 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="38"/>
-      <c r="B14" s="113">
+      <c r="B14" s="111">
         <v>3</v>
       </c>
-      <c r="C14" s="113" t="s">
+      <c r="C14" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D14" s="18" t="s">
@@ -18734,7 +18742,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G14,Trigger)</f>
         <v>42223</v>
       </c>
-      <c r="G14" s="120">
+      <c r="G14" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B14&amp;"M","mf",TRUE)</f>
         <v>42223</v>
       </c>
@@ -18769,10 +18777,10 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="38"/>
-      <c r="B15" s="113">
+      <c r="B15" s="111">
         <v>4</v>
       </c>
-      <c r="C15" s="113" t="s">
+      <c r="C15" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="18" t="s">
@@ -18785,7 +18793,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G15,Trigger)</f>
         <v>42254</v>
       </c>
-      <c r="G15" s="120">
+      <c r="G15" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B15&amp;"M","mf",TRUE)</f>
         <v>42254</v>
       </c>
@@ -18817,10 +18825,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="38"/>
-      <c r="B16" s="113">
+      <c r="B16" s="111">
         <v>5</v>
       </c>
-      <c r="C16" s="113" t="s">
+      <c r="C16" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D16" s="18" t="s">
@@ -18833,7 +18841,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G16,Trigger)</f>
         <v>42284</v>
       </c>
-      <c r="G16" s="120">
+      <c r="G16" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B16&amp;"M","mf",TRUE)</f>
         <v>42284</v>
       </c>
@@ -18865,10 +18873,10 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="38"/>
-      <c r="B17" s="113">
+      <c r="B17" s="111">
         <v>6</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C17" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -18881,7 +18889,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G17,Trigger)</f>
         <v>42317</v>
       </c>
-      <c r="G17" s="120">
+      <c r="G17" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B17&amp;"M","mf",TRUE)</f>
         <v>42317</v>
       </c>
@@ -18916,10 +18924,10 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
-      <c r="B18" s="113">
+      <c r="B18" s="111">
         <v>7</v>
       </c>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -18932,7 +18940,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G18,Trigger)</f>
         <v>42345</v>
       </c>
-      <c r="G18" s="120">
+      <c r="G18" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B18&amp;"M","mf",TRUE)</f>
         <v>42345</v>
       </c>
@@ -18964,10 +18972,10 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="38"/>
-      <c r="B19" s="113">
+      <c r="B19" s="111">
         <v>8</v>
       </c>
-      <c r="C19" s="113" t="s">
+      <c r="C19" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
@@ -18980,7 +18988,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G19,Trigger)</f>
         <v>42376</v>
       </c>
-      <c r="G19" s="120">
+      <c r="G19" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B19&amp;"M","mf",TRUE)</f>
         <v>42376</v>
       </c>
@@ -19020,8 +19028,8 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="38"/>
-      <c r="B20" s="115"/>
-      <c r="C20" s="115"/>
+      <c r="B20" s="113"/>
+      <c r="C20" s="113"/>
       <c r="D20" s="102" t="s">
         <v>23</v>
       </c>
@@ -19049,10 +19057,10 @@
         <v>HKD3M1Y=</v>
       </c>
       <c r="K20" s="49"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="117" t="str">
+      <c r="L20" s="114"/>
+      <c r="M20" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D20,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d5#0000</v>
+        <v>obj_00203#0001</v>
       </c>
       <c r="N20" s="75"/>
       <c r="O20" s="77" t="s">
@@ -19076,23 +19084,23 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="38"/>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="116"/>
       <c r="D21" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="119" t="s">
+      <c r="E21" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="120">
+      <c r="F21" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G21" s="120">
+      <c r="G21" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M21,F21,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H21" s="120">
+      <c r="H21" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M21,G21,Trigger)</f>
         <v>42681</v>
       </c>
@@ -19105,10 +19113,10 @@
         <v>HKD3M18M=</v>
       </c>
       <c r="K21" s="51"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="117" t="str">
+      <c r="L21" s="114"/>
+      <c r="M21" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D21,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e4#0000</v>
+        <v>obj_001e6#0001</v>
       </c>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -19126,23 +19134,23 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="38"/>
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
+      <c r="B22" s="116"/>
+      <c r="C22" s="116"/>
       <c r="D22" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="119" t="s">
+      <c r="E22" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="120">
+      <c r="F22" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G22" s="120">
+      <c r="G22" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M22,F22,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H22" s="120">
+      <c r="H22" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M22,G22,Trigger)</f>
         <v>42863</v>
       </c>
@@ -19155,10 +19163,10 @@
         <v>HKD3M2Y=</v>
       </c>
       <c r="K22" s="51"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="117" t="str">
+      <c r="L22" s="114"/>
+      <c r="M22" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e0#0000</v>
+        <v>obj_001ee#0001</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="79"/>
@@ -19176,23 +19184,23 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="38"/>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
       <c r="D23" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="119" t="s">
+      <c r="E23" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="120">
+      <c r="F23" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G23" s="120">
+      <c r="G23" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M23,F23,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H23" s="120">
+      <c r="H23" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M23,G23,Trigger)</f>
         <v>43227</v>
       </c>
@@ -19205,10 +19213,10 @@
         <v>HKD3M3Y=</v>
       </c>
       <c r="K23" s="51"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117" t="str">
+      <c r="L23" s="114"/>
+      <c r="M23" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001fe#0000</v>
+        <v>obj_001e8#0001</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -19226,23 +19234,23 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="38"/>
-      <c r="B24" s="118"/>
-      <c r="C24" s="118"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="120">
+      <c r="F24" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G24" s="120">
+      <c r="G24" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M24,F24,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H24" s="120">
+      <c r="H24" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M24,G24,Trigger)</f>
         <v>43591</v>
       </c>
@@ -19255,10 +19263,10 @@
         <v>HKD3M4Y=</v>
       </c>
       <c r="K24" s="51"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="117" t="str">
+      <c r="L24" s="114"/>
+      <c r="M24" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00206#0000</v>
+        <v>obj_001d9#0001</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -19276,23 +19284,23 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="38"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="118"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="116"/>
       <c r="D25" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="E25" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="120">
+      <c r="F25" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G25" s="120">
+      <c r="G25" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M25,F25,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H25" s="120">
+      <c r="H25" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M25,G25,Trigger)</f>
         <v>43957</v>
       </c>
@@ -19305,10 +19313,10 @@
         <v>HKD3M5Y=</v>
       </c>
       <c r="K25" s="51"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="117" t="str">
+      <c r="L25" s="114"/>
+      <c r="M25" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e8#0000</v>
+        <v>obj_00205#0001</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -19326,23 +19334,23 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="38"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="118"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
       <c r="D26" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="120">
+      <c r="F26" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G26" s="120">
+      <c r="G26" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M26,F26,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H26" s="120">
+      <c r="H26" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M26,G26,Trigger)</f>
         <v>44687</v>
       </c>
@@ -19355,10 +19363,10 @@
         <v>HKD3M7Y=</v>
       </c>
       <c r="K26" s="51"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="117" t="str">
+      <c r="L26" s="114"/>
+      <c r="M26" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d9#0000</v>
+        <v>obj_001d5#0001</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -19376,23 +19384,23 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="38"/>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="120">
+      <c r="F27" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G27" s="120">
+      <c r="G27" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M27,F27,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H27" s="120">
+      <c r="H27" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M27,G27,Trigger)</f>
         <v>45783</v>
       </c>
@@ -19405,10 +19413,10 @@
         <v>HKD3M10Y=</v>
       </c>
       <c r="K27" s="51"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="117" t="str">
+      <c r="L27" s="114"/>
+      <c r="M27" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c7#0000</v>
+        <v>obj_001db#0001</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -19426,23 +19434,23 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="38"/>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
       <c r="D28" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="119" t="s">
+      <c r="E28" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="120">
+      <c r="F28" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G28" s="120">
+      <c r="G28" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M28,F28,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H28" s="120">
+      <c r="H28" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M28,G28,Trigger)</f>
         <v>46513</v>
       </c>
@@ -19455,10 +19463,10 @@
         <v>HKD3M12Y=</v>
       </c>
       <c r="K28" s="51"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="117" t="str">
+      <c r="L28" s="114"/>
+      <c r="M28" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ec#0000</v>
+        <v>obj_001d6#0001</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -19476,39 +19484,39 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="38"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
       <c r="D29" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="122" t="s">
+      <c r="E29" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="123">
+      <c r="F29" s="121">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G29" s="123">
+      <c r="G29" s="121">
         <f>_xll.qlInterestRateIndexValueDate(M29,F29,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H29" s="123">
+      <c r="H29" s="121">
         <f>_xll.qlInterestRateIndexMaturity(M29,G29,Trigger)</f>
         <v>47609</v>
       </c>
-      <c r="I29" s="124">
+      <c r="I29" s="122">
         <f>_xll.qlIndexFixing(M29,F29,TRUE,AllTriggers)</f>
         <v>2.1700000000074708E-2</v>
       </c>
-      <c r="J29" s="125" t="str">
+      <c r="J29" s="123" t="str">
         <f>Contribution!M29</f>
         <v>HKD3M15Y=</v>
       </c>
-      <c r="K29" s="125"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="126" t="str">
+      <c r="K29" s="123"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="124" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d3#0000</v>
+        <v>obj_001d4#0001</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -22483,8 +22491,8 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="38"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="111"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23" t="s">
         <v>39</v>
@@ -22533,8 +22541,8 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="38"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
       <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
@@ -22565,7 +22573,7 @@
       <c r="L6" s="38"/>
       <c r="M6" s="78" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D6="ON",D6="TN",D6="SN"),"1D",IF(D6="SW","1W",D6)),0,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d1#0000</v>
+        <v>obj_001c5#0001</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="b">
@@ -22589,8 +22597,8 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
       <c r="D7" s="18" t="s">
         <v>78</v>
       </c>
@@ -22621,7 +22629,7 @@
       <c r="L7" s="38"/>
       <c r="M7" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D7="ON",D7="TN",D7="SN"),"1D",IF(D7="SW","1W",D7)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00204#0000</v>
+        <v>obj_00213#0001</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -22639,8 +22647,8 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="38"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
       <c r="D8" s="18" t="s">
         <v>16</v>
       </c>
@@ -22671,7 +22679,7 @@
       <c r="L8" s="38"/>
       <c r="M8" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D8="ON",D8="TN",D8="SN"),"1D",IF(D8="SW","1W",D8)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001cb#0000</v>
+        <v>obj_001ed#0001</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -22689,8 +22697,8 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="38"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
       <c r="D9" s="18" t="s">
         <v>17</v>
       </c>
@@ -22721,7 +22729,7 @@
       <c r="L9" s="38"/>
       <c r="M9" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D9="ON",D9="TN",D9="SN"),"1D",IF(D9="SW","1W",D9)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_00200#0000</v>
+        <v>obj_001ec#0001</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -22739,8 +22747,8 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="38"/>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
       <c r="D10" s="18" t="s">
         <v>18</v>
       </c>
@@ -22771,7 +22779,7 @@
       <c r="L10" s="38"/>
       <c r="M10" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D10="ON",D10="TN",D10="SN"),"1D",IF(D10="SW","1W",D10)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001f6#0000</v>
+        <v>obj_001d1#0001</v>
       </c>
       <c r="N10" s="75"/>
       <c r="O10" s="79"/>
@@ -22789,8 +22797,8 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="38"/>
-      <c r="B11" s="113"/>
-      <c r="C11" s="113"/>
+      <c r="B11" s="111"/>
+      <c r="C11" s="111"/>
       <c r="D11" s="18" t="s">
         <v>19</v>
       </c>
@@ -22821,7 +22829,7 @@
       <c r="L11" s="38"/>
       <c r="M11" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D11="ON",D11="TN",D11="SN"),"1D",IF(D11="SW","1W",D11)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001d7#0000</v>
+        <v>obj_0020e#0001</v>
       </c>
       <c r="N11" s="38"/>
       <c r="O11" s="79"/>
@@ -22839,8 +22847,8 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="38"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="111"/>
       <c r="D12" s="18" t="s">
         <v>20</v>
       </c>
@@ -22851,7 +22859,7 @@
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G12" s="120">
+      <c r="G12" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M12,F12,Trigger)</f>
         <v>42130</v>
       </c>
@@ -22871,7 +22879,7 @@
       <c r="L12" s="38"/>
       <c r="M12" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D12="ON",D12="TN",D12="SN"),"1D",IF(D12="SW","1W",D12)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001f2#0000</v>
+        <v>obj_001df#0001</v>
       </c>
       <c r="N12" s="38"/>
       <c r="O12" s="79"/>
@@ -22889,8 +22897,8 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="38"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="18" t="s">
         <v>21</v>
       </c>
@@ -22901,7 +22909,7 @@
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G13" s="120">
+      <c r="G13" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M13,F13,Trigger)</f>
         <v>42130</v>
       </c>
@@ -22921,7 +22929,7 @@
       <c r="L13" s="38"/>
       <c r="M13" s="27" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D13="ON",D13="TN",D13="SN"),"1D",IF(D13="SW","1W",D13)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001fd#0000</v>
+        <v>obj_00206#0001</v>
       </c>
       <c r="N13" s="38"/>
       <c r="O13" s="79"/>
@@ -22939,8 +22947,8 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="38"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
       <c r="D14" s="19" t="s">
         <v>14</v>
       </c>
@@ -22951,7 +22959,7 @@
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G14" s="123">
+      <c r="G14" s="121">
         <f>_xll.qlInterestRateIndexValueDate(M14,F14,Trigger)</f>
         <v>42130</v>
       </c>
@@ -22971,7 +22979,7 @@
       <c r="L14" s="38"/>
       <c r="M14" s="29" t="str">
         <f>_xll.qlIborIndex(,"Hibor",IF(OR(D14="ON",D14="TN",D14="SN"),"1D",IF(D14="SW","1W",D14)),SettlementDays,Currency,Calendar,BDayConvention,EndOfMonth,DayCounter,YieldCurve,,Trigger)</f>
-        <v>obj_001c9#0000</v>
+        <v>obj_001fe#0001</v>
       </c>
       <c r="N14" s="38"/>
       <c r="O14" s="79"/>
@@ -22989,10 +22997,10 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="38"/>
-      <c r="B15" s="112">
+      <c r="B15" s="110">
         <v>1</v>
       </c>
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="110" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="17" t="s">
@@ -23040,10 +23048,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="38"/>
-      <c r="B16" s="113">
+      <c r="B16" s="111">
         <v>2</v>
       </c>
-      <c r="C16" s="113" t="s">
+      <c r="C16" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D16" s="18" t="s">
@@ -23056,7 +23064,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G16,Trigger)</f>
         <v>42192</v>
       </c>
-      <c r="G16" s="120">
+      <c r="G16" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B16&amp;"M","mf",TRUE)</f>
         <v>42192</v>
       </c>
@@ -23091,10 +23099,10 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="38"/>
-      <c r="B17" s="113">
+      <c r="B17" s="111">
         <v>3</v>
       </c>
-      <c r="C17" s="113" t="s">
+      <c r="C17" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -23107,7 +23115,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G17,Trigger)</f>
         <v>42223</v>
       </c>
-      <c r="G17" s="120">
+      <c r="G17" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B17&amp;"M","mf",TRUE)</f>
         <v>42223</v>
       </c>
@@ -23142,10 +23150,10 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
-      <c r="B18" s="113">
+      <c r="B18" s="111">
         <v>4</v>
       </c>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -23158,7 +23166,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G18,Trigger)</f>
         <v>42254</v>
       </c>
-      <c r="G18" s="120">
+      <c r="G18" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B18&amp;"M","mf",TRUE)</f>
         <v>42254</v>
       </c>
@@ -23193,10 +23201,10 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="38"/>
-      <c r="B19" s="113">
+      <c r="B19" s="111">
         <v>5</v>
       </c>
-      <c r="C19" s="113" t="s">
+      <c r="C19" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
@@ -23209,7 +23217,7 @@
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G19,Trigger)</f>
         <v>42284</v>
       </c>
-      <c r="G19" s="120">
+      <c r="G19" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B19&amp;"M","mf",TRUE)</f>
         <v>42284</v>
       </c>
@@ -23244,10 +23252,10 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="38"/>
-      <c r="B20" s="118">
+      <c r="B20" s="116">
         <v>6</v>
       </c>
-      <c r="C20" s="113" t="s">
+      <c r="C20" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D20" s="103" t="s">
@@ -23256,15 +23264,15 @@
       <c r="E20" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="120">
+      <c r="F20" s="118">
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G20,Trigger)</f>
         <v>42317</v>
       </c>
-      <c r="G20" s="120">
+      <c r="G20" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B20&amp;"M","mf",TRUE)</f>
         <v>42317</v>
       </c>
-      <c r="H20" s="120">
+      <c r="H20" s="118">
         <f>_xll.qlInterestRateIndexMaturity(IborIndex,G20,Trigger)</f>
         <v>42499</v>
       </c>
@@ -23277,7 +23285,7 @@
         <v>HKD6M6X12F=</v>
       </c>
       <c r="K20" s="51"/>
-      <c r="L20" s="116"/>
+      <c r="L20" s="114"/>
       <c r="M20" s="75"/>
       <c r="N20" s="75"/>
       <c r="O20" s="79"/>
@@ -23295,10 +23303,10 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="38"/>
-      <c r="B21" s="118">
+      <c r="B21" s="116">
         <v>12</v>
       </c>
-      <c r="C21" s="113" t="s">
+      <c r="C21" s="111" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="103" t="s">
@@ -23307,15 +23315,15 @@
       <c r="E21" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="120">
+      <c r="F21" s="118">
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G21,Trigger)</f>
         <v>42499</v>
       </c>
-      <c r="G21" s="120">
+      <c r="G21" s="118">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B21&amp;"M","mf",TRUE)</f>
         <v>42499</v>
       </c>
-      <c r="H21" s="120">
+      <c r="H21" s="118">
         <f>_xll.qlInterestRateIndexMaturity(IborIndex,G21,Trigger)</f>
         <v>42683</v>
       </c>
@@ -23328,7 +23336,7 @@
         <v>HKD6M12X18F=</v>
       </c>
       <c r="K21" s="51"/>
-      <c r="L21" s="116"/>
+      <c r="L21" s="114"/>
       <c r="M21" s="75"/>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -23346,10 +23354,10 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="38"/>
-      <c r="B22" s="121">
+      <c r="B22" s="119">
         <v>18</v>
       </c>
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="112" t="s">
         <v>90</v>
       </c>
       <c r="D22" s="104" t="s">
@@ -23358,28 +23366,28 @@
       <c r="E22" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="123">
+      <c r="F22" s="121">
         <f>_xll.qlInterestRateIndexFixingDate(IborIndex,G22,Trigger)</f>
         <v>42681</v>
       </c>
-      <c r="G22" s="123">
+      <c r="G22" s="121">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","following",FALSE,Trigger),B22&amp;"M","mf",TRUE)</f>
         <v>42681</v>
       </c>
-      <c r="H22" s="123">
+      <c r="H22" s="121">
         <f>_xll.qlInterestRateIndexMaturity(IborIndex,G22,Trigger)</f>
         <v>42863</v>
       </c>
-      <c r="I22" s="124">
+      <c r="I22" s="122">
         <f>_xll.qlIndexFixing(IborIndex,F22,TRUE,AllTriggers)</f>
         <v>1.4000000000000051E-2</v>
       </c>
-      <c r="J22" s="125" t="str">
+      <c r="J22" s="123" t="str">
         <f>Contribution!Q22</f>
         <v>HKD6M18X24F=</v>
       </c>
-      <c r="K22" s="125"/>
-      <c r="L22" s="116"/>
+      <c r="K22" s="123"/>
+      <c r="L22" s="114"/>
       <c r="M22" s="76" t="s">
         <v>38</v>
       </c>
@@ -23405,23 +23413,23 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="38"/>
-      <c r="B23" s="118"/>
-      <c r="C23" s="118"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="116"/>
       <c r="D23" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="119" t="s">
+      <c r="E23" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="120">
+      <c r="F23" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G23" s="120">
+      <c r="G23" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M23,F23,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H23" s="120">
+      <c r="H23" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M23,G23,Trigger)</f>
         <v>43227</v>
       </c>
@@ -23434,10 +23442,10 @@
         <v>HKD6M3Y=</v>
       </c>
       <c r="K23" s="51"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117" t="str">
+      <c r="L23" s="114"/>
+      <c r="M23" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001fc#0000</v>
+        <v>obj_001f5#0001</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="77" t="s">
@@ -23461,23 +23469,23 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="38"/>
-      <c r="B24" s="118"/>
-      <c r="C24" s="118"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
       <c r="D24" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="120">
+      <c r="F24" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G24" s="120">
+      <c r="G24" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M24,F24,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H24" s="120">
+      <c r="H24" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M24,G24,Trigger)</f>
         <v>43591</v>
       </c>
@@ -23490,10 +23498,10 @@
         <v>HKD6M4Y=</v>
       </c>
       <c r="K24" s="51"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="117" t="str">
+      <c r="L24" s="114"/>
+      <c r="M24" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001cf#0000</v>
+        <v>obj_0020d#0001</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -23511,23 +23519,23 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="38"/>
-      <c r="B25" s="118"/>
-      <c r="C25" s="118"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="116"/>
       <c r="D25" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="E25" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="120">
+      <c r="F25" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G25" s="120">
+      <c r="G25" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M25,F25,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H25" s="120">
+      <c r="H25" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M25,G25,Trigger)</f>
         <v>43957</v>
       </c>
@@ -23540,10 +23548,10 @@
         <v>HKD6M5Y=</v>
       </c>
       <c r="K25" s="51"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="117" t="str">
+      <c r="L25" s="114"/>
+      <c r="M25" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f1#0000</v>
+        <v>obj_001ef#0001</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -23561,23 +23569,23 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="38"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="118"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
       <c r="D26" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="120">
+      <c r="F26" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G26" s="120">
+      <c r="G26" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M26,F26,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H26" s="120">
+      <c r="H26" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M26,G26,Trigger)</f>
         <v>44687</v>
       </c>
@@ -23590,10 +23598,10 @@
         <v>HKD6M7Y=</v>
       </c>
       <c r="K26" s="51"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="117" t="str">
+      <c r="L26" s="114"/>
+      <c r="M26" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001df#0000</v>
+        <v>obj_001ea#0001</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -23611,23 +23619,23 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="38"/>
-      <c r="B27" s="118"/>
-      <c r="C27" s="118"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="120">
+      <c r="F27" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G27" s="120">
+      <c r="G27" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M27,F27,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H27" s="120">
+      <c r="H27" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M27,G27,Trigger)</f>
         <v>45783</v>
       </c>
@@ -23640,10 +23648,10 @@
         <v>HKD6M10Y=</v>
       </c>
       <c r="K27" s="51"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="117" t="str">
+      <c r="L27" s="114"/>
+      <c r="M27" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d2#0000</v>
+        <v>obj_001e9#0001</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -23661,23 +23669,23 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="38"/>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
       <c r="D28" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="119" t="s">
+      <c r="E28" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="120">
+      <c r="F28" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G28" s="120">
+      <c r="G28" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M28,F28,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H28" s="120">
+      <c r="H28" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M28,G28,Trigger)</f>
         <v>46513</v>
       </c>
@@ -23690,10 +23698,10 @@
         <v>HKD6M12Y=</v>
       </c>
       <c r="K28" s="51"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="117" t="str">
+      <c r="L28" s="114"/>
+      <c r="M28" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001c8#0000</v>
+        <v>obj_00201#0001</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -23711,39 +23719,39 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="38"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
       <c r="D29" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="122" t="s">
+      <c r="E29" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="123">
+      <c r="F29" s="121">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G29" s="123">
+      <c r="G29" s="121">
         <f>_xll.qlInterestRateIndexValueDate(M29,F29,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H29" s="123">
+      <c r="H29" s="121">
         <f>_xll.qlInterestRateIndexMaturity(M29,G29,Trigger)</f>
         <v>47609</v>
       </c>
-      <c r="I29" s="124">
+      <c r="I29" s="122">
         <f>_xll.qlIndexFixing(M29,F29,TRUE,AllTriggers)</f>
         <v>1.3685088691286927E-2</v>
       </c>
-      <c r="J29" s="125" t="str">
+      <c r="J29" s="123" t="str">
         <f>Contribution!Q29</f>
         <v>HKD6M15Y=</v>
       </c>
-      <c r="K29" s="125"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="126" t="str">
+      <c r="K29" s="123"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="124" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d0#0000</v>
+        <v>obj_00209#0001</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -26671,7 +26679,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="29" t="str">
         <f>_xll.qlOvernightIndex(,"Honix",0,Currency,Calendar,"act/365 (fixed)",YieldCurve,,Trigger)</f>
-        <v>obj_001e5#0000</v>
+        <v>obj_001c7#0001</v>
       </c>
       <c r="N3" s="5"/>
       <c r="O3" s="79"/>
@@ -26794,9 +26802,9 @@
       <c r="J6" s="49"/>
       <c r="K6" s="50"/>
       <c r="L6" s="38"/>
-      <c r="M6" s="117" t="str">
+      <c r="M6" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D6="ON","1D",D6),SettlementDays,Currency,Calendar,FixedLegTenor,"Following",FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00207#0000</v>
+        <v>obj_001e0#0001</v>
       </c>
       <c r="N6" s="75"/>
       <c r="O6" s="77" t="s">
@@ -26825,7 +26833,7 @@
       <c r="D7" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="45">
@@ -26847,9 +26855,9 @@
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
       <c r="L7" s="38"/>
-      <c r="M7" s="117" t="str">
+      <c r="M7" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D7="ON","1D",D7),SettlementDays,Currency,Calendar,FixedLegTenor,"Following",FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00218#0000</v>
+        <v>obj_00216#0001</v>
       </c>
       <c r="N7" s="75"/>
       <c r="O7" s="79"/>
@@ -26872,7 +26880,7 @@
       <c r="D8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="119" t="s">
+      <c r="E8" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="45">
@@ -26894,9 +26902,9 @@
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="38"/>
-      <c r="M8" s="117" t="str">
+      <c r="M8" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D8="ON","1D",D8),SettlementDays,Currency,Calendar,FixedLegTenor,"Following",FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e6#0000</v>
+        <v>obj_001d0#0001</v>
       </c>
       <c r="N8" s="75"/>
       <c r="O8" s="79"/>
@@ -26919,7 +26927,7 @@
       <c r="D9" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="119" t="s">
+      <c r="E9" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="45">
@@ -26944,9 +26952,9 @@
       </c>
       <c r="K9" s="35"/>
       <c r="L9" s="38"/>
-      <c r="M9" s="117" t="str">
+      <c r="M9" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D9="ON","1D",D9),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00212#0000</v>
+        <v>obj_001cf#0001</v>
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="79"/>
@@ -26969,7 +26977,7 @@
       <c r="D10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="119" t="s">
+      <c r="E10" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="45">
@@ -26994,9 +27002,9 @@
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="38"/>
-      <c r="M10" s="117" t="str">
+      <c r="M10" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D10="ON","1D",D10),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020d#0000</v>
+        <v>obj_001f6#0001</v>
       </c>
       <c r="N10" s="75"/>
       <c r="O10" s="79"/>
@@ -27019,7 +27027,7 @@
       <c r="D11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="45">
@@ -27044,9 +27052,9 @@
       </c>
       <c r="K11" s="35"/>
       <c r="L11" s="38"/>
-      <c r="M11" s="117" t="str">
+      <c r="M11" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D11="ON","1D",D11),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f7#0000</v>
+        <v>obj_001d7#0001</v>
       </c>
       <c r="N11" s="75"/>
       <c r="O11" s="79"/>
@@ -27069,14 +27077,14 @@
       <c r="D12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="119" t="s">
+      <c r="E12" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G12" s="120">
+      <c r="G12" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M12,F12,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27094,9 +27102,9 @@
       </c>
       <c r="K12" s="35"/>
       <c r="L12" s="38"/>
-      <c r="M12" s="117" t="str">
+      <c r="M12" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D12="ON","1D",D12),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00214#0000</v>
+        <v>obj_001da#0001</v>
       </c>
       <c r="N12" s="75"/>
       <c r="O12" s="79"/>
@@ -27119,14 +27127,14 @@
       <c r="D13" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="119" t="s">
+      <c r="E13" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G13" s="120">
+      <c r="G13" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M13,F13,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27144,9 +27152,9 @@
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="38"/>
-      <c r="M13" s="117" t="str">
+      <c r="M13" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D13="ON","1D",D13),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e7#0000</v>
+        <v>obj_001de#0001</v>
       </c>
       <c r="N13" s="75"/>
       <c r="O13" s="79"/>
@@ -27169,14 +27177,14 @@
       <c r="D14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="119" t="s">
+      <c r="E14" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G14" s="120">
+      <c r="G14" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M14,F14,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27194,9 +27202,9 @@
       </c>
       <c r="K14" s="35"/>
       <c r="L14" s="38"/>
-      <c r="M14" s="117" t="str">
+      <c r="M14" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D14="ON","1D",D14),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00211#0000</v>
+        <v>obj_001fd#0001</v>
       </c>
       <c r="N14" s="75"/>
       <c r="O14" s="79"/>
@@ -27219,14 +27227,14 @@
       <c r="D15" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="119" t="s">
+      <c r="E15" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G15" s="120">
+      <c r="G15" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M15,F15,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27241,9 +27249,9 @@
       <c r="J15" s="35"/>
       <c r="K15" s="35"/>
       <c r="L15" s="38"/>
-      <c r="M15" s="117" t="str">
+      <c r="M15" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D15="ON","1D",D15),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f5#0000</v>
+        <v>obj_001ca#0001</v>
       </c>
       <c r="N15" s="75"/>
       <c r="O15" s="79"/>
@@ -27266,14 +27274,14 @@
       <c r="D16" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="119" t="s">
+      <c r="E16" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G16" s="120">
+      <c r="G16" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M16,F16,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27288,9 +27296,9 @@
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
       <c r="L16" s="38"/>
-      <c r="M16" s="117" t="str">
+      <c r="M16" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D16="ON","1D",D16),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0021a#0000</v>
+        <v>obj_00219#0001</v>
       </c>
       <c r="N16" s="75"/>
       <c r="O16" s="79"/>
@@ -27313,14 +27321,14 @@
       <c r="D17" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="119" t="s">
+      <c r="E17" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G17" s="120">
+      <c r="G17" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M17,F17,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27338,9 +27346,9 @@
       </c>
       <c r="K17" s="35"/>
       <c r="L17" s="38"/>
-      <c r="M17" s="117" t="str">
+      <c r="M17" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D17="ON","1D",D17),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020e#0000</v>
+        <v>obj_001e3#0001</v>
       </c>
       <c r="N17" s="75"/>
       <c r="O17" s="79"/>
@@ -27363,14 +27371,14 @@
       <c r="D18" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="119" t="s">
+      <c r="E18" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G18" s="120">
+      <c r="G18" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M18,F18,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27385,9 +27393,9 @@
       <c r="J18" s="35"/>
       <c r="K18" s="35"/>
       <c r="L18" s="38"/>
-      <c r="M18" s="117" t="str">
+      <c r="M18" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D18="ON","1D",D18),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00203#0000</v>
+        <v>obj_001e5#0001</v>
       </c>
       <c r="N18" s="75"/>
       <c r="O18" s="79"/>
@@ -27410,14 +27418,14 @@
       <c r="D19" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="45">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G19" s="120">
+      <c r="G19" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M19,F19,Trigger)</f>
         <v>42130</v>
       </c>
@@ -27432,9 +27440,9 @@
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
       <c r="L19" s="38"/>
-      <c r="M19" s="117" t="str">
+      <c r="M19" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D19="ON","1D",D19),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00205#0000</v>
+        <v>obj_001cd#0001</v>
       </c>
       <c r="N19" s="75"/>
       <c r="O19" s="79"/>
@@ -27457,18 +27465,18 @@
       <c r="D20" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="120">
+      <c r="F20" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G20" s="120">
+      <c r="G20" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M20,F20,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H20" s="120">
+      <c r="H20" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M20,G20,Trigger)</f>
         <v>42496</v>
       </c>
@@ -27481,10 +27489,10 @@
         <v>HKDOIS1YD=</v>
       </c>
       <c r="K20" s="51"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="117" t="str">
+      <c r="L20" s="114"/>
+      <c r="M20" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D20="ON","1D",D20),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00210#0000</v>
+        <v>obj_00215#0001</v>
       </c>
       <c r="N20" s="75"/>
       <c r="O20" s="79"/>
@@ -27507,18 +27515,18 @@
       <c r="D21" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="119" t="s">
+      <c r="E21" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="120">
+      <c r="F21" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G21" s="120">
+      <c r="G21" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M21,F21,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H21" s="120">
+      <c r="H21" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M21,G21,Trigger)</f>
         <v>42681</v>
       </c>
@@ -27531,10 +27539,10 @@
         <v>HKDOIS18MD=</v>
       </c>
       <c r="K21" s="51"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="117" t="str">
+      <c r="L21" s="114"/>
+      <c r="M21" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D21="ON","1D",D21),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020f#0000</v>
+        <v>obj_001fb#0001</v>
       </c>
       <c r="N21" s="75"/>
       <c r="O21" s="79"/>
@@ -27557,18 +27565,18 @@
       <c r="D22" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="119" t="s">
+      <c r="E22" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="120">
+      <c r="F22" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G22" s="120">
+      <c r="G22" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M22,F22,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H22" s="120">
+      <c r="H22" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M22,G22,Trigger)</f>
         <v>42863</v>
       </c>
@@ -27581,10 +27589,10 @@
         <v>HKDOIS2YD=</v>
       </c>
       <c r="K22" s="51"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="117" t="str">
+      <c r="L22" s="114"/>
+      <c r="M22" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D22="ON","1D",D22),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00213#0000</v>
+        <v>obj_001d2#0001</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="79"/>
@@ -27607,18 +27615,18 @@
       <c r="D23" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="119" t="s">
+      <c r="E23" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="120">
+      <c r="F23" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G23" s="120">
+      <c r="G23" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M23,F23,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H23" s="120">
+      <c r="H23" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M23,G23,Trigger)</f>
         <v>43227</v>
       </c>
@@ -27631,10 +27639,10 @@
         <v>HKDOIS3YD=</v>
       </c>
       <c r="K23" s="51"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117" t="str">
+      <c r="L23" s="114"/>
+      <c r="M23" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D23="ON","1D",D23),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ed#0000</v>
+        <v>obj_00207#0001</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -27657,18 +27665,18 @@
       <c r="D24" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="120">
+      <c r="F24" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G24" s="120">
+      <c r="G24" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M24,F24,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H24" s="120">
+      <c r="H24" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M24,G24,Trigger)</f>
         <v>43591</v>
       </c>
@@ -27681,10 +27689,10 @@
         <v>HKDOIS4YD=</v>
       </c>
       <c r="K24" s="51"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="117" t="str">
+      <c r="L24" s="114"/>
+      <c r="M24" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D24="ON","1D",D24),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00202#0000</v>
+        <v>obj_001f7#0001</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -27707,18 +27715,18 @@
       <c r="D25" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="E25" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="120">
+      <c r="F25" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G25" s="120">
+      <c r="G25" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M25,F25,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H25" s="120">
+      <c r="H25" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M25,G25,Trigger)</f>
         <v>43957</v>
       </c>
@@ -27731,10 +27739,10 @@
         <v>HKDOIS5YD=</v>
       </c>
       <c r="K25" s="51"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="117" t="str">
+      <c r="L25" s="114"/>
+      <c r="M25" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D25="ON","1D",D25),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ea#0000</v>
+        <v>obj_0020a#0001</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -27757,18 +27765,18 @@
       <c r="D26" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="120">
+      <c r="F26" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G26" s="120">
+      <c r="G26" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M26,F26,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H26" s="120">
+      <c r="H26" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M26,G26,Trigger)</f>
         <v>44687</v>
       </c>
@@ -27781,10 +27789,10 @@
         <v>HKDOIS7YD=</v>
       </c>
       <c r="K26" s="51"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="117" t="str">
+      <c r="L26" s="114"/>
+      <c r="M26" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D26="ON","1D",D26),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00216#0000</v>
+        <v>obj_001f8#0001</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -27807,18 +27815,18 @@
       <c r="D27" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="120">
+      <c r="F27" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G27" s="120">
+      <c r="G27" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M27,F27,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H27" s="120">
+      <c r="H27" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M27,G27,Trigger)</f>
         <v>45783</v>
       </c>
@@ -27831,10 +27839,10 @@
         <v>HKDOIS10YD=</v>
       </c>
       <c r="K27" s="51"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="117" t="str">
+      <c r="L27" s="114"/>
+      <c r="M27" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D27="ON","1D",D27),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00217#0000</v>
+        <v>obj_00208#0001</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -27857,18 +27865,18 @@
       <c r="D28" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="119" t="s">
+      <c r="E28" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="120">
+      <c r="F28" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G28" s="120">
+      <c r="G28" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M28,F28,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H28" s="120">
+      <c r="H28" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M28,G28,Trigger)</f>
         <v>46513</v>
       </c>
@@ -27881,10 +27889,10 @@
         <v>HKDOIS12YD=</v>
       </c>
       <c r="K28" s="51"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="117" t="str">
+      <c r="L28" s="114"/>
+      <c r="M28" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D28="ON","1D",D28),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_00215#0000</v>
+        <v>obj_001e1#0001</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -27907,18 +27915,18 @@
       <c r="D29" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="122" t="s">
+      <c r="E29" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="123">
+      <c r="F29" s="121">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G29" s="123">
+      <c r="G29" s="121">
         <f>_xll.qlInterestRateIndexValueDate(M29,F29,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H29" s="123">
+      <c r="H29" s="121">
         <f>_xll.qlInterestRateIndexMaturity(M29,G29,Trigger)</f>
         <v>47609</v>
       </c>
@@ -27926,15 +27934,15 @@
         <f>_xll.qlIndexFixing(M29,F29,TRUE,AllTriggers)</f>
         <v>#NUM!</v>
       </c>
-      <c r="J29" s="125" t="str">
+      <c r="J29" s="123" t="str">
         <f>Contribution!U29</f>
         <v>HKDOIS15YD=</v>
       </c>
-      <c r="K29" s="125"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="126" t="str">
+      <c r="K29" s="123"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="124" t="str">
         <f>_xll.qlSwapIndex(,"Honix",IF(D29="ON","1D",D29),SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,OvernightIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020c#0000</v>
+        <v>obj_001f1#0001</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -28013,7 +28021,7 @@
       <c r="D32" s="3"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="131"/>
+      <c r="G32" s="129"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -28069,7 +28077,7 @@
       <c r="D34" s="3"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="131"/>
+      <c r="G34" s="129"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -28125,7 +28133,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="131"/>
+      <c r="G36" s="129"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
@@ -28181,7 +28189,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="131"/>
+      <c r="G38" s="129"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
@@ -28237,7 +28245,7 @@
       <c r="D40" s="3"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="131"/>
+      <c r="G40" s="129"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -28293,7 +28301,7 @@
       <c r="D42" s="3"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="131"/>
+      <c r="G42" s="129"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
@@ -28349,7 +28357,7 @@
       <c r="D44" s="3"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="131"/>
+      <c r="G44" s="129"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
@@ -28405,7 +28413,7 @@
       <c r="D46" s="3"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="131"/>
+      <c r="G46" s="129"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
@@ -28461,7 +28469,7 @@
       <c r="D48" s="3"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="131"/>
+      <c r="G48" s="129"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
@@ -31137,7 +31145,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="26"/>
       <c r="F12" s="45"/>
-      <c r="G12" s="120"/>
+      <c r="G12" s="118"/>
       <c r="H12" s="45"/>
       <c r="I12" s="44"/>
       <c r="J12" s="35"/>
@@ -31165,7 +31173,7 @@
       <c r="D13" s="18"/>
       <c r="E13" s="26"/>
       <c r="F13" s="45"/>
-      <c r="G13" s="120"/>
+      <c r="G13" s="118"/>
       <c r="H13" s="45"/>
       <c r="I13" s="44"/>
       <c r="J13" s="35"/>
@@ -31193,7 +31201,7 @@
       <c r="D14" s="18"/>
       <c r="E14" s="26"/>
       <c r="F14" s="45"/>
-      <c r="G14" s="120"/>
+      <c r="G14" s="118"/>
       <c r="H14" s="45"/>
       <c r="I14" s="44"/>
       <c r="J14" s="35"/>
@@ -31221,7 +31229,7 @@
       <c r="D15" s="18"/>
       <c r="E15" s="26"/>
       <c r="F15" s="45"/>
-      <c r="G15" s="120"/>
+      <c r="G15" s="118"/>
       <c r="H15" s="45"/>
       <c r="I15" s="44"/>
       <c r="J15" s="35"/>
@@ -31249,7 +31257,7 @@
       <c r="D16" s="18"/>
       <c r="E16" s="26"/>
       <c r="F16" s="45"/>
-      <c r="G16" s="120"/>
+      <c r="G16" s="118"/>
       <c r="H16" s="45"/>
       <c r="I16" s="44"/>
       <c r="J16" s="35"/>
@@ -31277,7 +31285,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="26"/>
       <c r="F17" s="45"/>
-      <c r="G17" s="120"/>
+      <c r="G17" s="118"/>
       <c r="H17" s="45"/>
       <c r="I17" s="44"/>
       <c r="J17" s="35"/>
@@ -31305,7 +31313,7 @@
       <c r="D18" s="18"/>
       <c r="E18" s="26"/>
       <c r="F18" s="45"/>
-      <c r="G18" s="120"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="45"/>
       <c r="I18" s="44"/>
       <c r="J18" s="35"/>
@@ -31333,7 +31341,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="26"/>
       <c r="F19" s="45"/>
-      <c r="G19" s="120"/>
+      <c r="G19" s="118"/>
       <c r="H19" s="45"/>
       <c r="I19" s="44"/>
       <c r="J19" s="35"/>
@@ -31360,13 +31368,13 @@
       <c r="C20" s="38"/>
       <c r="D20" s="103"/>
       <c r="E20" s="26"/>
-      <c r="F20" s="120"/>
-      <c r="G20" s="120"/>
-      <c r="H20" s="120"/>
+      <c r="F20" s="118"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="118"/>
       <c r="I20" s="96"/>
       <c r="J20" s="51"/>
       <c r="K20" s="51"/>
-      <c r="L20" s="116"/>
+      <c r="L20" s="114"/>
       <c r="M20" s="79"/>
       <c r="N20" s="79"/>
       <c r="O20" s="79"/>
@@ -31388,13 +31396,13 @@
       <c r="C21" s="38"/>
       <c r="D21" s="104"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="124"/>
-      <c r="J21" s="125"/>
-      <c r="K21" s="125"/>
-      <c r="L21" s="116"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="121"/>
+      <c r="H21" s="121"/>
+      <c r="I21" s="122"/>
+      <c r="J21" s="123"/>
+      <c r="K21" s="123"/>
+      <c r="L21" s="114"/>
       <c r="M21" s="76" t="s">
         <v>38</v>
       </c>
@@ -31449,10 +31457,10 @@
         <v>HKDSTD2Y=</v>
       </c>
       <c r="K22" s="49"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="117" t="str">
+      <c r="L22" s="114"/>
+      <c r="M22" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D22,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001cc#0000</v>
+        <v>obj_001dc#0001</v>
       </c>
       <c r="N22" s="75"/>
       <c r="O22" s="77" t="s">
@@ -31481,18 +31489,18 @@
       <c r="D23" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="119" t="s">
+      <c r="E23" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="120">
+      <c r="F23" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G23" s="120">
+      <c r="G23" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M23,F23,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H23" s="120">
+      <c r="H23" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M23,G23,Trigger)</f>
         <v>43227</v>
       </c>
@@ -31505,10 +31513,10 @@
         <v>HKDSTD3Y=</v>
       </c>
       <c r="K23" s="51"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="117" t="str">
+      <c r="L23" s="114"/>
+      <c r="M23" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D23,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f8#0000</v>
+        <v>obj_001f4#0001</v>
       </c>
       <c r="N23" s="75"/>
       <c r="O23" s="79"/>
@@ -31531,18 +31539,18 @@
       <c r="D24" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="120">
+      <c r="F24" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G24" s="120">
+      <c r="G24" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M24,F24,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H24" s="120">
+      <c r="H24" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M24,G24,Trigger)</f>
         <v>43591</v>
       </c>
@@ -31555,10 +31563,10 @@
         <v>HKDSTD4Y=</v>
       </c>
       <c r="K24" s="51"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="117" t="str">
+      <c r="L24" s="114"/>
+      <c r="M24" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D24,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001f4#0000</v>
+        <v>obj_00218#0001</v>
       </c>
       <c r="N24" s="75"/>
       <c r="O24" s="79"/>
@@ -31581,18 +31589,18 @@
       <c r="D25" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="E25" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="120">
+      <c r="F25" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G25" s="120">
+      <c r="G25" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M25,F25,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H25" s="120">
+      <c r="H25" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M25,G25,Trigger)</f>
         <v>43957</v>
       </c>
@@ -31605,10 +31613,10 @@
         <v>HKDSTD5Y=</v>
       </c>
       <c r="K25" s="51"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="117" t="str">
+      <c r="L25" s="114"/>
+      <c r="M25" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D25,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001d8#0000</v>
+        <v>obj_001fc#0001</v>
       </c>
       <c r="N25" s="75"/>
       <c r="O25" s="79"/>
@@ -31631,18 +31639,18 @@
       <c r="D26" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="120">
+      <c r="F26" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G26" s="120">
+      <c r="G26" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M26,F26,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H26" s="120">
+      <c r="H26" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M26,G26,Trigger)</f>
         <v>44687</v>
       </c>
@@ -31655,10 +31663,10 @@
         <v>HKDSTD7Y=</v>
       </c>
       <c r="K26" s="51"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="117" t="str">
+      <c r="L26" s="114"/>
+      <c r="M26" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D26,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001ff#0000</v>
+        <v>obj_001cc#0001</v>
       </c>
       <c r="N26" s="75"/>
       <c r="O26" s="79"/>
@@ -31681,18 +31689,18 @@
       <c r="D27" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="119" t="s">
+      <c r="E27" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="120">
+      <c r="F27" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G27" s="120">
+      <c r="G27" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M27,F27,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H27" s="120">
+      <c r="H27" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M27,G27,Trigger)</f>
         <v>45783</v>
       </c>
@@ -31705,10 +31713,10 @@
         <v>HKDSTD10Y=</v>
       </c>
       <c r="K27" s="51"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="117" t="str">
+      <c r="L27" s="114"/>
+      <c r="M27" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D27,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_0020a#0000</v>
+        <v>obj_0020b#0001</v>
       </c>
       <c r="N27" s="75"/>
       <c r="O27" s="79"/>
@@ -31731,18 +31739,18 @@
       <c r="D28" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="119" t="s">
+      <c r="E28" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="120">
+      <c r="F28" s="118">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G28" s="120">
+      <c r="G28" s="118">
         <f>_xll.qlInterestRateIndexValueDate(M28,F28,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H28" s="120">
+      <c r="H28" s="118">
         <f>_xll.qlInterestRateIndexMaturity(M28,G28,Trigger)</f>
         <v>46513</v>
       </c>
@@ -31755,10 +31763,10 @@
         <v>HKDSTD12Y=</v>
       </c>
       <c r="K28" s="51"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="117" t="str">
+      <c r="L28" s="114"/>
+      <c r="M28" s="115" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D28,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001e3#0000</v>
+        <v>obj_00210#0001</v>
       </c>
       <c r="N28" s="75"/>
       <c r="O28" s="79"/>
@@ -31781,34 +31789,34 @@
       <c r="D29" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="122" t="s">
+      <c r="E29" s="120" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="123">
+      <c r="F29" s="121">
         <f t="shared" si="0"/>
         <v>42129</v>
       </c>
-      <c r="G29" s="123">
+      <c r="G29" s="121">
         <f>_xll.qlInterestRateIndexValueDate(M29,F29,Trigger)</f>
         <v>42130</v>
       </c>
-      <c r="H29" s="123">
+      <c r="H29" s="121">
         <f>_xll.qlInterestRateIndexMaturity(M29,G29,Trigger)</f>
         <v>47609</v>
       </c>
-      <c r="I29" s="124">
+      <c r="I29" s="122">
         <f>_xll.qlIndexFixing(M29,F29,TRUE,AllTriggers)</f>
         <v>2.1700000000074708E-2</v>
       </c>
-      <c r="J29" s="125" t="str">
+      <c r="J29" s="123" t="str">
         <f>Contribution!Y29</f>
         <v>HKDSTD15Y=</v>
       </c>
-      <c r="K29" s="125"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="126" t="str">
+      <c r="K29" s="123"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="124" t="str">
         <f>_xll.qlSwapIndex(,"Hibor",D29,SettlementDays,Currency,Calendar,FixedLegTenor,FixedLegBDC,FixedLegDayCounter,IborIndex,YieldCurve,,Trigger)</f>
-        <v>obj_001fa#0000</v>
+        <v>obj_001cb#0001</v>
       </c>
       <c r="N29" s="75"/>
       <c r="O29" s="79"/>
@@ -31862,7 +31870,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="127"/>
+      <c r="J31" s="125"/>
       <c r="K31" s="5"/>
       <c r="L31" s="38"/>
       <c r="M31" s="79"/>
@@ -31890,7 +31898,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="127"/>
+      <c r="J32" s="125"/>
       <c r="K32" s="5"/>
       <c r="L32" s="38"/>
       <c r="M32" s="79"/>
@@ -31918,7 +31926,7 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="127"/>
+      <c r="J33" s="125"/>
       <c r="K33" s="5"/>
       <c r="L33" s="38"/>
       <c r="M33" s="79"/>
@@ -31946,8 +31954,8 @@
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="127"/>
-      <c r="K34" s="130"/>
+      <c r="J34" s="125"/>
+      <c r="K34" s="128"/>
       <c r="L34" s="38"/>
       <c r="M34" s="79"/>
       <c r="N34" s="75"/>
@@ -31974,8 +31982,8 @@
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="127"/>
-      <c r="K35" s="130"/>
+      <c r="J35" s="125"/>
+      <c r="K35" s="128"/>
       <c r="L35" s="38"/>
       <c r="M35" s="79"/>
       <c r="N35" s="75"/>
@@ -32002,8 +32010,8 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="127"/>
-      <c r="K36" s="130"/>
+      <c r="J36" s="125"/>
+      <c r="K36" s="128"/>
       <c r="L36" s="38"/>
       <c r="M36" s="79"/>
       <c r="N36" s="75"/>
@@ -32030,8 +32038,8 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="127"/>
-      <c r="K37" s="130"/>
+      <c r="J37" s="125"/>
+      <c r="K37" s="128"/>
       <c r="L37" s="38"/>
       <c r="M37" s="79"/>
       <c r="N37" s="79"/>
@@ -32058,8 +32066,8 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="127"/>
-      <c r="K38" s="130"/>
+      <c r="J38" s="125"/>
+      <c r="K38" s="128"/>
       <c r="L38" s="38"/>
       <c r="M38" s="79"/>
       <c r="N38" s="79"/>
@@ -32087,7 +32095,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
-      <c r="K39" s="130"/>
+      <c r="K39" s="128"/>
       <c r="L39" s="79"/>
       <c r="M39" s="79"/>
       <c r="N39" s="79"/>
@@ -32115,7 +32123,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="130"/>
+      <c r="K40" s="128"/>
       <c r="L40" s="79"/>
       <c r="M40" s="79"/>
       <c r="N40" s="79"/>
@@ -32143,7 +32151,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="130"/>
+      <c r="K41" s="128"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>

</xml_diff>